<commit_message>
added mon - fri
</commit_message>
<xml_diff>
--- a/zoom_meets.xlsx
+++ b/zoom_meets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEIL\PycharmProjects\zoom_auto_join\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B0DA5-1611-47F9-87B8-F84A16B255EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020AA535-96AA-4FE5-B84F-236C06C2CB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25890" yWindow="10245" windowWidth="21600" windowHeight="11430" xr2:uid="{7AD01A05-5E8D-4C8E-B311-F48B5E90C4B6}"/>
+    <workbookView xWindow="1972" yWindow="1448" windowWidth="8356" windowHeight="7792" xr2:uid="{7AD01A05-5E8D-4C8E-B311-F48B5E90C4B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>meet_name</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>zoom.com/STSWENG</t>
+  </si>
+  <si>
+    <t>T Th</t>
+  </si>
+  <si>
+    <t>T F</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -562,7 +568,7 @@
         <v>0.53125</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -576,7 +582,7 @@
         <v>0.53125</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>